<commit_message>
ChangeOwner - Revised disclosureType when changing into company owner.
</commit_message>
<xml_diff>
--- a/skrum_docs/04_SpecificDesign/11_OKRDetails_公開範囲設定画面仕様書_20170702.xlsx
+++ b/skrum_docs/04_SpecificDesign/11_OKRDetails_公開範囲設定画面仕様書_20170702.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/OneDrive/Skrum/07_プロダクト開発/プロダクト資料/03_詳細設計/画面仕様書/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/Dev/skrum/skrum_docs/04_SpecificDesign/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -506,8 +506,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4089400" y="2197100"/>
-          <a:ext cx="9550400" cy="1244600"/>
+          <a:off x="4080847" y="2225092"/>
+          <a:ext cx="9524741" cy="1270518"/>
           <a:chOff x="4089400" y="2006600"/>
           <a:chExt cx="9550400" cy="1244600"/>
         </a:xfrm>
@@ -773,16 +773,76 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>362858</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12959</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>544287</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>129592</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="正方形/長方形 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10509899" y="4121020"/>
+          <a:ext cx="1308878" cy="635001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>642258</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>223158</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -791,8 +851,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13347700" y="3568700"/>
-          <a:ext cx="2971800" cy="1524000"/>
+          <a:off x="11916748" y="3627793"/>
+          <a:ext cx="2963247" cy="1555102"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -829,6 +889,186 @@
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" baseline="0"/>
             <a:t> defined by 'disclosureType' of the okr.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>846496</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>73866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1023776</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>90715</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="四角形吹き出し 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="846496" y="553356"/>
+          <a:ext cx="2432178" cy="1053583"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -46229"/>
+            <a:gd name="adj2" fmla="val -22158"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>In</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" baseline="0"/>
+            <a:t> case that the owner is user or group.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>116633</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>207347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>643690</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>155511</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3498980" y="10276633"/>
+          <a:ext cx="7291751" cy="6168572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>816429</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>207346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>993709</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>224195</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="四角形吹き出し 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="816429" y="10276632"/>
+          <a:ext cx="2432178" cy="1053583"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -46229"/>
+            <a:gd name="adj2" fmla="val -22158"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>In</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" baseline="0"/>
+            <a:t> case that the owner is company.</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
         </a:p>
@@ -1104,9 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>